<commit_message>
Edited GroupPlana and Little Changes to LoginButton and LoginPane
</commit_message>
<xml_diff>
--- a/doc/GroupPlan.xlsx
+++ b/doc/GroupPlan.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{75AB7D64-D88C-489C-843E-BA019B6C18D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CamposDev\Workspace-Github\CSE248\ParkingGarageProject\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238CB454-CFC9-462A-9D13-052C8506D729}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="23280" windowHeight="16035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -67,9 +64,6 @@
     <t>3 hours</t>
   </si>
   <si>
-    <t>MenuBar</t>
-  </si>
-  <si>
     <t xml:space="preserve">HistoryPane (gui) </t>
   </si>
   <si>
@@ -134,6 +128,9 @@
   </si>
   <si>
     <t>700 minutes</t>
+  </si>
+  <si>
+    <t>GarageMenuBar</t>
   </si>
 </sst>
 </file>
@@ -705,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="98" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="98" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,7 +799,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3">
         <v>60</v>
@@ -810,7 +807,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3">
         <v>60</v>
@@ -818,7 +815,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3">
         <v>60</v>
@@ -826,7 +823,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="3">
         <v>45</v>
@@ -835,12 +832,12 @@
         <v>13</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3">
         <v>120</v>
@@ -848,31 +845,31 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="3">
         <v>180</v>
@@ -886,15 +883,15 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" s="3">
         <v>90</v>
@@ -905,7 +902,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="3">
         <v>20</v>
@@ -913,18 +910,18 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3">
         <v>20</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3">
         <v>30</v>
@@ -932,15 +929,15 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="3">
         <v>120</v>
@@ -948,13 +945,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited GroupPlan (InsertUserPane and LoginPane is Green)
</commit_message>
<xml_diff>
--- a/doc/GroupPlan.xlsx
+++ b/doc/GroupPlan.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7CC39811-F34D-4F19-AFDA-DCDB2F6F845B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CamposDev\Workspace-Github\CSE248\ParkingGarageProject\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C9C12F-7355-48FB-A482-9C5F39496B1A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="23280" windowHeight="16035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -100,12 +97,6 @@
     <t>ImgUtil</t>
   </si>
   <si>
-    <t>CheckInPane (Extends TabPane?)</t>
-  </si>
-  <si>
-    <t>CheckOutPane(extends Tab)</t>
-  </si>
-  <si>
     <t>LightWork</t>
   </si>
   <si>
@@ -134,6 +125,12 @@
   </si>
   <si>
     <t>700 minutes</t>
+  </si>
+  <si>
+    <t>CheckInPane</t>
+  </si>
+  <si>
+    <t>CheckOutPane</t>
   </si>
 </sst>
 </file>
@@ -714,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="98" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="98" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,7 +799,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3">
@@ -810,8 +807,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>28</v>
+      <c r="A10" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B10" s="3">
         <v>60</v>
@@ -819,7 +816,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B11" s="3">
         <v>60</v>
@@ -827,7 +824,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3">
         <v>60</v>
@@ -835,7 +832,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3">
         <v>45</v>
@@ -844,7 +841,7 @@
         <v>13</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -881,7 +878,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" s="3">
         <v>180</v>
@@ -941,15 +938,15 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3">
         <v>120</v>
@@ -957,13 +954,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made Some Changes to GroupPlan (Used Formula)
</commit_message>
<xml_diff>
--- a/doc/GroupPlan.xlsx
+++ b/doc/GroupPlan.xlsx
@@ -3,20 +3,31 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C8E124E9-28A9-4F26-8325-D45379CDDFAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CamposDev\Workspace-Github\CSE248\ParkingGarageProject\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCC5AAB-A223-47BF-B18E-9E1BF77D8E80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21660" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Class/Design of Project</t>
   </si>
@@ -118,9 +129,6 @@
   </si>
   <si>
     <t>490 minutes</t>
-  </si>
-  <si>
-    <t>700 minutes</t>
   </si>
   <si>
     <t>CheckInPane</t>
@@ -176,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +219,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -241,7 +255,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -265,6 +279,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -713,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="98" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,7 +835,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3">
         <v>60</v>
@@ -826,7 +843,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3">
         <v>60</v>
@@ -883,13 +900,13 @@
         <v>27</v>
       </c>
       <c r="B18" s="3">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="C18" s="8">
         <v>120</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -939,22 +956,25 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="9" t="s">
         <v>28</v>
+      </c>
+      <c r="B24" s="3">
+        <v>120</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>37</v>
+      <c r="A25" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="B25" s="3">
         <v>50</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="3">
         <v>45</v>
@@ -962,7 +982,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3">
         <v>45</v>
@@ -973,12 +993,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="3">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>34</v>
+      <c r="B28" s="3">
+        <f>SUM(B3:B27)</f>
+        <v>660</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Edited GroupPlan (Calculated Total Work Time)
</commit_message>
<xml_diff>
--- a/doc/GroupPlan.xlsx
+++ b/doc/GroupPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CamposDev\Workspace-Github\CSE248\ParkingGarageProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCC5AAB-A223-47BF-B18E-9E1BF77D8E80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA36A25-347E-4A06-837F-364EB28E6D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Class/Design of Project</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Space (holds Vehicle and d)</t>
   </si>
   <si>
-    <t>~30</t>
-  </si>
-  <si>
     <t>Parking Lot (array of Space) ArrayList</t>
   </si>
   <si>
@@ -68,27 +65,15 @@
     <t>LoginPane</t>
   </si>
   <si>
-    <t>3 hours</t>
-  </si>
-  <si>
-    <t>MenuBar</t>
-  </si>
-  <si>
     <t xml:space="preserve">HistoryPane (gui) </t>
   </si>
   <si>
-    <t>20minutes</t>
-  </si>
-  <si>
     <t>History Data (Day Logs) - LinkedList&lt;T&gt; (.data files)</t>
   </si>
   <si>
     <t>UserData</t>
   </si>
   <si>
-    <t>20 minutes</t>
-  </si>
-  <si>
     <t>Save Data (Parking Spaces + Users + Invoices)</t>
   </si>
   <si>
@@ -116,21 +101,12 @@
     <t>Javadoc work</t>
   </si>
   <si>
-    <t>~100</t>
-  </si>
-  <si>
-    <t>&gt;600 minutes</t>
-  </si>
-  <si>
     <t>ListViewOccupiedSpaces(gui) *</t>
   </si>
   <si>
     <t>*- Not doing 'open' tickets.</t>
   </si>
   <si>
-    <t>490 minutes</t>
-  </si>
-  <si>
     <t>CheckInPane</t>
   </si>
   <si>
@@ -140,20 +116,38 @@
     <t>Debugging GUI merge with backcode + General Debugging</t>
   </si>
   <si>
-    <t>120 (General DB)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reworking UML Class Diagram </t>
   </si>
   <si>
-    <t>30 minutes</t>
+    <t>GarageMenuBar</t>
+  </si>
+  <si>
+    <t>LoginButton</t>
+  </si>
+  <si>
+    <t>ViewGarageButton</t>
+  </si>
+  <si>
+    <t>DeleteUserDialog</t>
+  </si>
+  <si>
+    <t>MainMenuPane</t>
+  </si>
+  <si>
+    <t>MainStage</t>
+  </si>
+  <si>
+    <t>UserDataViewer</t>
+  </si>
+  <si>
+    <t>&lt;---- (Minutes)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,8 +177,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,12 +201,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59996337778862885"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -275,13 +271,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -728,18 +724,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="98" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" style="3" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="3"/>
     <col min="8" max="8" width="22.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -747,7 +743,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -764,46 +760,46 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
+      <c r="C2" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>30</v>
       </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C6" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3">
         <v>90</v>
@@ -811,39 +807,39 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
         <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>12</v>
+      <c r="A9" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>26</v>
+      <c r="A10" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B10" s="3">
         <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>34</v>
+      <c r="A11" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="3">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>35</v>
+      <c r="A12" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="B12" s="3">
         <v>60</v>
@@ -851,21 +847,21 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="7">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6">
         <v>45</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>13</v>
+      <c r="D13" s="3">
+        <v>180</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>14</v>
+      <c r="A14" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B14" s="3">
         <v>120</v>
@@ -873,53 +869,53 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
+      </c>
+      <c r="D15" s="3">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="D16" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="D17" s="3">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>27</v>
+      <c r="A18" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B18" s="3">
         <v>60</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>120</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
+      <c r="D18" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3">
         <v>20</v>
       </c>
-      <c r="D19" s="3" t="s">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="C20" s="3">
         <v>90</v>
@@ -929,52 +925,49 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>22</v>
+      <c r="A21" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="B21" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="B22" s="3">
-        <v>20</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="B24" s="3">
         <v>120</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>29</v>
+      <c r="C24" s="6">
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>36</v>
+      <c r="A25" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B25" s="3">
         <v>50</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>37</v>
+      <c r="C25" s="3">
+        <v>120</v>
       </c>
       <c r="D25" s="3">
         <v>45</v>
@@ -982,30 +975,83 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C26" s="3">
         <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>25</v>
+      <c r="A27" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B27" s="3">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="B28" s="3">
-        <f>SUM(B3:B27)</f>
-        <v>660</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>33</v>
+      </c>
+      <c r="B30" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
+        <f>SUM(B2:B33)</f>
+        <v>940</v>
+      </c>
+      <c r="C34" s="3">
+        <f>SUM(C2:C33)</f>
+        <v>850</v>
+      </c>
+      <c r="D34" s="3">
+        <f>SUM(D2:D33)</f>
+        <v>435</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>